<commit_message>
Update source code and exe version 1. = DEBUG exe version 1.02 = Without DEBUG
</commit_message>
<xml_diff>
--- a/AutoCorrectAPI/Data_Compare_ชื่อบริษัท.xlsx
+++ b/AutoCorrectAPI/Data_Compare_ชื่อบริษัท.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1fastaccess\RPA\RPA_source\Information Retrieval\iEditDistance\AutoCorrectAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3E0572-2E88-40F4-80EE-62DC55C76B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDACBFCB-35A4-43C9-B769-3BB03244E24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{33AD17F5-1DCF-48CF-8E38-550215D1E0A5}"/>
   </bookViews>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F527A7F6-2A2E-4FAE-80B1-D0DBE7FDA597}">
   <dimension ref="A1:A179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:XFD82"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A180" sqref="A180:XFD180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,37 +1797,37 @@
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>